<commit_message>
Transformation du dataframe pour récupérer les infos clefs
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,32 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://elevacap.sharepoint.com/sites/ELEVA_Solutions/Shared Documents/General/Victor B/articles &amp; recherche/code/SRP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="11_94CD5ADFF0FD93CA5F1F5F07CF540A88FBD4AD6C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF66596F-84E7-49F2-8B6B-C0AD49D142DE}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_145F63B9AFD473300EF588D67633A5EFB5A1E6B0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C19C650E-C86E-4060-AC2A-5835C349C22A}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-240" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="184">
   <si>
     <t>Id</t>
   </si>
@@ -209,6 +196,33 @@
     <t>PotentialMaxPayout</t>
   </si>
   <si>
+    <t>PDI_Type_</t>
+  </si>
+  <si>
+    <t>PDI_Barrier_</t>
+  </si>
+  <si>
+    <t>ISIN_</t>
+  </si>
+  <si>
+    <t>Issuer_</t>
+  </si>
+  <si>
+    <t>Country_</t>
+  </si>
+  <si>
+    <t>Distributor_</t>
+  </si>
+  <si>
+    <t>FT_</t>
+  </si>
+  <si>
+    <t>AssetClass_</t>
+  </si>
+  <si>
+    <t>Underlying_</t>
+  </si>
+  <si>
     <t>NotFlow</t>
   </si>
   <si>
@@ -308,6 +322,30 @@
     <t>2025-08-29T14:23:50Z</t>
   </si>
   <si>
+    <t>European</t>
+  </si>
+  <si>
+    <t>XS3127061219</t>
+  </si>
+  <si>
+    <t>Citi</t>
+  </si>
+  <si>
+    <t>FRA</t>
+  </si>
+  <si>
+    <t>Non-public</t>
+  </si>
+  <si>
+    <t>https://brochures.structuredretailproducts.com/brochure/2025/08/29/71-14-5F-D4-4F-DF-B3-DD-F1-E1-E8-30-A4-53-0C-AB.pdf</t>
+  </si>
+  <si>
+    <t>Equity (Single Index)</t>
+  </si>
+  <si>
+    <t>MerQube NORDEA BANK ABP 0.94 Point Decrement EUR Index</t>
+  </si>
+  <si>
     <t>Growth</t>
   </si>
   <si>
@@ -362,6 +400,15 @@
     <t>Autocall Securities linked to an Index</t>
   </si>
   <si>
+    <t>XS3127110446</t>
+  </si>
+  <si>
+    <t>https://brochures.structuredretailproducts.com/brochure/2025/08/29/1A-5D-E5-DC-C3-1D-E5-67-B1-38-F6-29-88-D9-28-54.pdf</t>
+  </si>
+  <si>
+    <t>MerQube Repsol SA 0.975 Point Decrement EUR Index</t>
+  </si>
+  <si>
     <t>2035-01-08T00:00:00Z</t>
   </si>
   <si>
@@ -407,6 +454,15 @@
     <t>AAAAAAQsR1o=</t>
   </si>
   <si>
+    <t>XS2965541464</t>
+  </si>
+  <si>
+    <t>https://brochures.structuredretailproducts.com/brochure/2025/08/29/14-A4-AF-3D-39-12-93-86-FF-D3-7B-F5-F5-01-52-C0.pdf</t>
+  </si>
+  <si>
+    <t>MerQube BNP 4.6 Index Point Decrement EUR Index</t>
+  </si>
+  <si>
     <t>2029-05-03T00:00:00Z</t>
   </si>
   <si>
@@ -458,6 +514,18 @@
     <t>Worst of Memory Coupon Barrier Autocall Notes</t>
   </si>
   <si>
+    <t>XS2807754440</t>
+  </si>
+  <si>
+    <t>https://brochures.structuredretailproducts.com/brochure/2025/08/29/85-E4-82-08-D6-AF-0B-D9-16-D1-9C-88-65-3F-1F-36.pdf</t>
+  </si>
+  <si>
+    <t>Equity (Share Basket)</t>
+  </si>
+  <si>
+    <t>Renault</t>
+  </si>
+  <si>
     <t>2035-10-10T00:00:00Z</t>
   </si>
   <si>
@@ -495,6 +563,15 @@
   </si>
   <si>
     <t>AAAAAAQsR1M=</t>
+  </si>
+  <si>
+    <t>FRC764200271</t>
+  </si>
+  <si>
+    <t>https://brochures.structuredretailproducts.com/brochure/2025/08/29/10-51-BA-9C-70-25-80-3E-FF-0A-86-44-5F-28-02-DA.pdf</t>
+  </si>
+  <si>
+    <t>Morningstar Developed Europe Energy Select 10 Decrement 50 Point GR EUR Index</t>
   </si>
 </sst>
 </file>
@@ -515,24 +592,12 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -562,15 +627,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -875,56 +934,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BF15"/>
+  <dimension ref="A1:BO6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AE15" sqref="AE15"/>
+    <sheetView tabSelected="1" topLeftCell="AV1" workbookViewId="0">
+      <selection activeCell="BO7" sqref="BO7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="26.7109375" customWidth="1"/>
-    <col min="7" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28" customWidth="1"/>
-    <col min="14" max="14" width="66.7109375" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" customWidth="1"/>
-    <col min="16" max="16" width="30.140625" customWidth="1"/>
-    <col min="17" max="17" width="122" customWidth="1"/>
-    <col min="18" max="18" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="25" customWidth="1"/>
-    <col min="21" max="21" width="23.85546875" customWidth="1"/>
-    <col min="22" max="22" width="24.5703125" customWidth="1"/>
-    <col min="23" max="23" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.85546875" customWidth="1"/>
-    <col min="25" max="25" width="107.85546875" customWidth="1"/>
-    <col min="26" max="26" width="28.28515625" customWidth="1"/>
-    <col min="27" max="27" width="86.85546875" customWidth="1"/>
-    <col min="28" max="28" width="255.5703125" customWidth="1"/>
-    <col min="29" max="29" width="30" customWidth="1"/>
-    <col min="33" max="34" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="18" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="42" max="43" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="15" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="6" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="54" max="55" width="53" bestFit="1" customWidth="1"/>
-    <col min="56" max="57" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="168.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -936,58 +961,58 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="W1" s="1" t="s">
@@ -999,13 +1024,13 @@
       <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
       <c r="AC1" s="1" t="s">
@@ -1020,7 +1045,7 @@
       <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AG1" s="1" t="s">
         <v>32</v>
       </c>
       <c r="AH1" s="1" t="s">
@@ -1047,7 +1072,7 @@
       <c r="AO1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AP1" s="1" t="s">
         <v>41</v>
       </c>
       <c r="AQ1" s="1" t="s">
@@ -1086,7 +1111,7 @@
       <c r="BB1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="2" t="s">
+      <c r="BC1" s="1" t="s">
         <v>54</v>
       </c>
       <c r="BD1" s="1" t="s">
@@ -1098,40 +1123,67 @@
       <c r="BF1" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="BG1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>54187698</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="G2" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="H2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="I2" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="J2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="K2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="L2">
         <v>12.23014</v>
@@ -1140,109 +1192,109 @@
         <v>12.23014</v>
       </c>
       <c r="N2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="O2" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="P2" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="Q2" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="R2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="S2" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="T2" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="U2" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="V2" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="W2" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="X2" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="Y2" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="Z2" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="AA2" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="AB2" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="AC2" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="AD2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AE2" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="AF2" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="AG2" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="AH2" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="AI2">
         <v>0</v>
       </c>
       <c r="AJ2" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="AK2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AL2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="AM2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AN2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AO2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AP2" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="AQ2" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="AR2" t="b">
         <v>0</v>
       </c>
       <c r="AS2" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="AT2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AU2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AV2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AX2" t="b">
         <v>1</v>
@@ -1254,54 +1306,81 @@
         <v>1</v>
       </c>
       <c r="BA2" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="BB2" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="BC2" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="BD2" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="BE2" t="s">
-        <v>90</v>
+        <v>99</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>100</v>
+      </c>
+      <c r="BH2">
+        <v>-50</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>101</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>102</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>103</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>104</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>105</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>106</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>54187693</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="E3" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="G3" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="H3" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="I3" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="J3" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="K3" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="L3">
         <v>12.0274</v>
@@ -1310,109 +1389,109 @@
         <v>12.0274</v>
       </c>
       <c r="N3" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="O3" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="P3" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="Q3" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="R3" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="S3" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="T3" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="U3" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="V3" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="W3" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="X3" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="Y3" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="Z3" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="AA3" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="AB3" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="AC3" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="AD3" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AE3" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="AF3" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="AG3" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AH3" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="AI3">
         <v>0</v>
       </c>
       <c r="AJ3" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="AK3" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AL3" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="AM3" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AN3" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AO3" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AP3" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="AQ3" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="AR3" t="b">
         <v>0</v>
       </c>
       <c r="AS3" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="AT3" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AU3" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AV3" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AX3" t="b">
         <v>1</v>
@@ -1424,54 +1503,81 @@
         <v>1</v>
       </c>
       <c r="BA3" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="BB3" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="BC3" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="BD3" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="BE3" t="s">
-        <v>90</v>
+        <v>99</v>
+      </c>
+      <c r="BG3" t="s">
+        <v>100</v>
+      </c>
+      <c r="BH3">
+        <v>-40</v>
+      </c>
+      <c r="BI3" t="s">
+        <v>126</v>
+      </c>
+      <c r="BJ3" t="s">
+        <v>102</v>
+      </c>
+      <c r="BK3" t="s">
+        <v>103</v>
+      </c>
+      <c r="BL3" t="s">
+        <v>104</v>
+      </c>
+      <c r="BM3" t="s">
+        <v>127</v>
+      </c>
+      <c r="BN3" t="s">
+        <v>106</v>
+      </c>
+      <c r="BO3" t="s">
+        <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>54187696</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="F4" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="G4" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="H4" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="I4" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
       <c r="J4" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="K4" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="L4">
         <v>10.0274</v>
@@ -1480,109 +1586,109 @@
         <v>10.0274</v>
       </c>
       <c r="N4" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="O4" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="P4" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
       <c r="Q4" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="R4" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="S4" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="T4" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="U4" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="V4" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="W4" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="X4" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="Y4" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="Z4" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="AA4" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="AB4" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="AC4" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
       <c r="AD4" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AE4" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="AF4" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="AG4" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="AH4" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="AI4">
         <v>0</v>
       </c>
       <c r="AJ4" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="AK4" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AL4" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="AM4" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AN4" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AO4" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AP4" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="AQ4" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="AR4" t="b">
         <v>0</v>
       </c>
       <c r="AS4" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
       <c r="AT4" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AU4" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AV4" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AX4" t="b">
         <v>1</v>
@@ -1594,54 +1700,81 @@
         <v>1</v>
       </c>
       <c r="BA4" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="BB4" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="BC4" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="BD4" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="BE4" t="s">
-        <v>90</v>
+        <v>99</v>
+      </c>
+      <c r="BG4" t="s">
+        <v>100</v>
+      </c>
+      <c r="BH4">
+        <v>-50</v>
+      </c>
+      <c r="BI4" t="s">
+        <v>144</v>
+      </c>
+      <c r="BJ4" t="s">
+        <v>102</v>
+      </c>
+      <c r="BK4" t="s">
+        <v>103</v>
+      </c>
+      <c r="BL4" t="s">
+        <v>104</v>
+      </c>
+      <c r="BM4" t="s">
+        <v>145</v>
+      </c>
+      <c r="BN4" t="s">
+        <v>106</v>
+      </c>
+      <c r="BO4" t="s">
+        <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>54187697</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="F5" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="G5" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="H5" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="I5" t="s">
-        <v>126</v>
+        <v>149</v>
       </c>
       <c r="J5" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="K5" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="L5">
         <v>5.0219199999999997</v>
@@ -1650,109 +1783,109 @@
         <v>5.0219199999999997</v>
       </c>
       <c r="N5" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="O5" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="P5" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="Q5" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="R5" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="S5" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="T5" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="U5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="V5" t="s">
-        <v>129</v>
+        <v>152</v>
       </c>
       <c r="W5" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="X5" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="Y5" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
       <c r="Z5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="AA5" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="AB5" t="s">
-        <v>132</v>
+        <v>155</v>
       </c>
       <c r="AC5" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="AD5" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AE5" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="AF5" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="AG5" t="s">
-        <v>134</v>
+        <v>157</v>
       </c>
       <c r="AH5" t="s">
-        <v>135</v>
+        <v>158</v>
       </c>
       <c r="AI5">
         <v>0</v>
       </c>
       <c r="AJ5" t="s">
-        <v>136</v>
+        <v>159</v>
       </c>
       <c r="AK5" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AL5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="AM5" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AN5" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AO5" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AP5" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="AQ5" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="AR5" t="b">
         <v>0</v>
       </c>
       <c r="AS5" t="s">
-        <v>138</v>
+        <v>161</v>
       </c>
       <c r="AT5" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AU5" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AV5" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AX5" t="b">
         <v>1</v>
@@ -1764,54 +1897,81 @@
         <v>1</v>
       </c>
       <c r="BA5" t="s">
-        <v>139</v>
+        <v>162</v>
       </c>
       <c r="BB5" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="BC5" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="BD5" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="BE5" t="s">
-        <v>90</v>
+        <v>99</v>
+      </c>
+      <c r="BG5" t="s">
+        <v>100</v>
+      </c>
+      <c r="BH5">
+        <v>-50</v>
+      </c>
+      <c r="BI5" t="s">
+        <v>164</v>
+      </c>
+      <c r="BJ5" t="s">
+        <v>102</v>
+      </c>
+      <c r="BK5" t="s">
+        <v>103</v>
+      </c>
+      <c r="BL5" t="s">
+        <v>104</v>
+      </c>
+      <c r="BM5" t="s">
+        <v>165</v>
+      </c>
+      <c r="BN5" t="s">
+        <v>166</v>
+      </c>
+      <c r="BO5" t="s">
+        <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>54187689</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="E6" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="F6" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="G6" t="s">
-        <v>141</v>
+        <v>168</v>
       </c>
       <c r="H6" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="I6" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="J6" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="K6" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="L6">
         <v>10.241099999999999</v>
@@ -1820,109 +1980,109 @@
         <v>10.241099999999999</v>
       </c>
       <c r="N6" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="O6" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="P6" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="Q6" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="R6" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="S6" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="T6" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="U6" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="V6" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="W6" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="X6" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="Y6" t="s">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="Z6" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="AA6" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="AB6" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="AC6" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="AD6" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AE6" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="AF6" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="AG6" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AH6" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="AI6">
         <v>0</v>
       </c>
       <c r="AJ6" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="AK6" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AL6" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="AM6" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AN6" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AO6" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AP6" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="AQ6" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="AR6" t="b">
         <v>0</v>
       </c>
       <c r="AS6" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
       <c r="AT6" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AU6" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AV6" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AX6" t="b">
         <v>1</v>
@@ -1934,25 +2094,46 @@
         <v>1</v>
       </c>
       <c r="BA6" t="s">
-        <v>153</v>
+        <v>180</v>
       </c>
       <c r="BB6" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="BC6" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="BD6" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="BE6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="AE15">
-        <f>154.81/135.65-1</f>
-        <v>0.14124585329893113</v>
+        <v>99</v>
+      </c>
+      <c r="BG6" t="s">
+        <v>100</v>
+      </c>
+      <c r="BH6">
+        <v>-50</v>
+      </c>
+      <c r="BI6" t="s">
+        <v>181</v>
+      </c>
+      <c r="BJ6" t="s">
+        <v>102</v>
+      </c>
+      <c r="BK6" t="s">
+        <v>103</v>
+      </c>
+      <c r="BL6" t="s">
+        <v>104</v>
+      </c>
+      <c r="BM6" t="s">
+        <v>182</v>
+      </c>
+      <c r="BN6" t="s">
+        <v>106</v>
+      </c>
+      <c r="BO6" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -2198,10 +2379,10 @@
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
-    <TaxCatchAll xmlns="4337af48-3994-435b-8794-88ffe27a10ca" xsi:nil="true"/>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="4bccb889-79a9-45e2-86ee-4a580dd6049d">
       <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="4337af48-3994-435b-8794-88ffe27a10ca" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
 </file>
@@ -2216,7 +2397,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0890AB0-51B9-4266-8EE3-2504E387ABDA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B53D491B-91F4-4F51-8E3D-4DB5DABE51B5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -2235,18 +2416,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AA6D26A-FEEF-4669-9E71-6E9B5F134AE1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B9A0197-B5B8-49AE-972F-8F3BFEBC466B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4bccb889-79a9-45e2-86ee-4a580dd6049d"/>
     <ds:schemaRef ds:uri="4337af48-3994-435b-8794-88ffe27a10ca"/>
-    <ds:schemaRef ds:uri="4bccb889-79a9-45e2-86ee-4a580dd6049d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4E11793-E38C-46A4-BDBC-92E317723E9F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75FF8DCE-6CEB-4F5F-8094-9D0193378018}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>

</xml_diff>